<commit_message>
log_output 갱신, description 최신화
</commit_message>
<xml_diff>
--- a/13조 UseCase description 1.xlsx
+++ b/13조 UseCase description 1.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC7E30ED-4607-426C-B2F4-31FDBA78373B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SW_engineering_13_group\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C70B5E52-E7FF-497D-890E-582FF13D9578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="122">
   <si>
     <t>Use Case Description</t>
   </si>
@@ -68,10 +73,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>6. 회원 정보 저장, 가입완료 메시지 출력. 로그인, 회원 가입 메뉴를 출력한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>회원 탈퇴</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -96,10 +97,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>8. 회원 탈퇴 메시지 출력, 시스템 접속을 종료한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>로그인</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -113,10 +110,6 @@
   </si>
   <si>
     <t>7. 로그아웃 메뉴를 누른다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>8. 로그아웃 메시지 출력, 시스템 접속을 종료한다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -300,15 +293,6 @@
     <t>9. 사용자가 이용 정보(결제 수단, 대여시간 등)를 입력 및 설정한다.</t>
   </si>
   <si>
-    <t>11. 대여 완료 되었다는 메시지를 띄운다.</t>
-  </si>
-  <si>
-    <t>12. 문자 알림 전송 서비스에게 대여 완료 알림을 요청한다.</t>
-  </si>
-  <si>
-    <t>13. 문자 알림 전송 서비스가 회원에게 알림 문자를 보낸다.</t>
-  </si>
-  <si>
     <t>대여중인 자전거 리스트 조회</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -321,27 +305,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>9. 대여중인 특정 자전거를 반납하려는 경우, 원하는 자전거의 반납 버튼을 누른다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10. 사용자 위치 정보 기반 근처 식당 추천 여부 메시지를 출력한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11. 근처 식당 추천 버튼을 누른다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>12. 식당 추천 및 예약 서비스를 제공한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Extension
-Step 8 이후, 회원은 대여중인 자전거를 반납할 수 있다.
-step 10 이후, 회원은 근처 식당을 추천 받을 수 있다.</t>
-  </si>
-  <si>
     <t>예약 대기 정보 조회</t>
   </si>
   <si>
@@ -352,9 +315,6 @@
   </si>
   <si>
     <t>9. 원하는 예약 대기의 취소 버튼을 누른다.</t>
-  </si>
-  <si>
-    <t>10. 예약 대기 취소 후, 예약 대기 취소 완료 메세지를 출력한다.</t>
   </si>
   <si>
     <t>Extension
@@ -444,13 +404,95 @@
   <si>
     <t>Extension
 Step 8 이후, 관리자는 조회 기간을 최근 1주일, 1개월, 1년 단위로 변경 가능</t>
+  </si>
+  <si>
+    <t>12. 문자 알림 전송 서비스가 회원에게 알림 문자를 보낸다.</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>6. 가입완료 메시지 출력. 로그인, 회원 가입 메뉴를 띄운다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8. 회원 탈퇴 메시지 출력. 로그인, 회원 가입 메뉴를 띄운다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10. 예약 대기 취소 후, 예약 대기 취소 완료 메세지를 출력한다.</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>9. 대여중인 특정 자전거를 반납하려는 경우, 원하는 자전거의 반납 버튼을 누른다.</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>8. 로그아웃 메시지 출력, 로그인, 회원 가입 메뉴를 띄운다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11. 예약 1순위 회원이 있는 때 이메일을 보낸다.</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>External Actor Action(이메일 서비스)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">10. 대기 예약한 회원 이메일 서비스와 연결한다. </t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">12. 요금 결제 서비스와 연결한다. </t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>10. 대여 완료 되었다는 메시지를 띄운다.</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>11. 문자 알림 전송 서비스에게 대여 완료 알림을 요청한다.</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>13. 회원이 사용한 자전거에 대한 요금을 결제한다.</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>14. 반납 완료 메시지와 사용자 위치 정보 기반 근처 식당 추천 여부 메시지를 출력한다.</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>15. 근처 식당 추천 버튼을 누른다.</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>16. 식당 추천 및 예약 외부 서비스와 연결한다.</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>17. 식당 추천 및 예약 서비스를 제공한다.</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Extension
+Step 8 이후, 회원은 대여중인 자전거를 반납할 수 있다.
+step 14 이후, 회원은 근처 식당을 추천 받을 수 있다.</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>External Actor Action(요금결제 서비스)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>External Actor Action(식당 추천 서비스)</t>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -495,6 +537,20 @@
       <family val="1"/>
       <charset val="129"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -510,7 +566,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -598,11 +654,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -650,16 +717,32 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -994,31 +1077,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C164"/>
+  <dimension ref="A1:E166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="B164" sqref="A158:B164"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="D118" sqref="D118"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40" customWidth="1"/>
-    <col min="2" max="2" width="45" customWidth="1"/>
+    <col min="1" max="1" width="41.875" customWidth="1"/>
+    <col min="2" max="2" width="50.375" customWidth="1"/>
     <col min="3" max="3" width="47.5" customWidth="1"/>
+    <col min="4" max="4" width="42.25" customWidth="1"/>
+    <col min="5" max="5" width="33.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="3"/>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -1026,7 +1111,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -1034,7 +1119,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
@@ -1042,21 +1127,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="34.5">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="B9" s="3"/>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>2</v>
       </c>
@@ -1064,7 +1149,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>4</v>
       </c>
@@ -1072,37 +1157,37 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="4" t="s">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="4" t="s">
+      <c r="B13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="4" t="s">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="8" t="s">
+      <c r="B14" s="8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="B16" s="3"/>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>2</v>
       </c>
@@ -1110,7 +1195,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>4</v>
       </c>
@@ -1118,29 +1203,29 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="4" t="s">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="4" t="s">
-        <v>13</v>
-      </c>
       <c r="B20" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B22" s="3"/>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>2</v>
       </c>
@@ -1148,7 +1233,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>4</v>
       </c>
@@ -1156,37 +1241,37 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="4" t="s">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="4" t="s">
-        <v>13</v>
-      </c>
       <c r="B26" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="8" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="8" t="s">
-        <v>20</v>
-      </c>
       <c r="B27" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B29" s="3"/>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>2</v>
       </c>
@@ -1194,7 +1279,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>4</v>
       </c>
@@ -1202,45 +1287,45 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B32" s="4" t="s">
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="4" t="s">
-        <v>13</v>
-      </c>
       <c r="B33" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="28.5" x14ac:dyDescent="0.3">
+      <c r="A35" s="8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="8" t="s">
+      <c r="B35" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B34" s="8" t="s">
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" ht="34.5">
-      <c r="A35" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="B37" s="3"/>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>2</v>
       </c>
@@ -1248,7 +1333,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>4</v>
       </c>
@@ -1256,51 +1341,51 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B40" s="4" t="s">
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="4" t="s">
-        <v>13</v>
-      </c>
       <c r="B41" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="28.5" x14ac:dyDescent="0.3">
+      <c r="A43" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B43" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B42" s="8" t="s">
+    </row>
+    <row r="44" spans="1:2" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="18" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" ht="34.5">
-      <c r="A43" s="8" t="s">
+      <c r="B44" s="19"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="33" customHeight="1">
-      <c r="A44" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B44" s="19"/>
-    </row>
-    <row r="46" spans="1:2">
-      <c r="A46" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="B46" s="3"/>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
         <v>2</v>
       </c>
@@ -1308,7 +1393,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>4</v>
       </c>
@@ -1316,45 +1401,45 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B49" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B49" s="4" t="s">
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="50" spans="1:2">
-      <c r="A50" s="4" t="s">
-        <v>13</v>
-      </c>
       <c r="B50" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B51" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="28.5" x14ac:dyDescent="0.3">
+      <c r="A52" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" ht="34.5">
-      <c r="A52" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2">
-      <c r="A54" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="B54" s="3"/>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
         <v>2</v>
       </c>
@@ -1362,7 +1447,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
         <v>4</v>
       </c>
@@ -1370,45 +1455,45 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B57" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B57" s="4" t="s">
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="58" spans="1:2">
-      <c r="A58" s="4" t="s">
-        <v>13</v>
-      </c>
       <c r="B58" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="28.5" x14ac:dyDescent="0.3">
+      <c r="A60" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B60" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B59" s="8" t="s">
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" ht="34.5">
-      <c r="A60" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B60" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2">
-      <c r="A62" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="B62" s="3"/>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
         <v>2</v>
       </c>
@@ -1416,7 +1501,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
         <v>4</v>
       </c>
@@ -1424,51 +1509,51 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B65" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B65" s="4" t="s">
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="66" spans="1:2">
-      <c r="A66" s="4" t="s">
-        <v>13</v>
-      </c>
       <c r="B66" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="28.5" x14ac:dyDescent="0.3">
+      <c r="A68" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B68" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B67" s="8" t="s">
+    </row>
+    <row r="69" spans="1:2" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="18" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" ht="34.5">
-      <c r="A68" s="8" t="s">
+      <c r="B69" s="19"/>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B68" s="8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" ht="32.25" customHeight="1">
-      <c r="A69" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="B69" s="19"/>
-    </row>
-    <row r="71" spans="1:2">
-      <c r="A71" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="B71" s="3"/>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="4" t="s">
         <v>2</v>
       </c>
@@ -1476,7 +1561,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="4" t="s">
         <v>4</v>
       </c>
@@ -1484,45 +1569,45 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B74" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B74" s="4" t="s">
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="75" spans="1:2">
-      <c r="A75" s="4" t="s">
-        <v>13</v>
-      </c>
       <c r="B75" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" ht="51">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="42.75" x14ac:dyDescent="0.3">
       <c r="A77" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B79" s="3"/>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="4" t="s">
         <v>2</v>
       </c>
@@ -1530,7 +1615,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="4" t="s">
         <v>4</v>
       </c>
@@ -1538,45 +1623,45 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B82" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B82" s="4" t="s">
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="83" spans="1:3">
-      <c r="A83" s="4" t="s">
-        <v>13</v>
-      </c>
       <c r="B83" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B84" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" s="8" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="84" spans="1:3">
-      <c r="A84" s="8" t="s">
+      <c r="B85" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B84" s="8" t="s">
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="85" spans="1:3">
-      <c r="A85" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="B85" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3">
-      <c r="A87" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="B87" s="3"/>
     </row>
-    <row r="88" spans="1:3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="4" t="s">
         <v>2</v>
       </c>
@@ -1584,10 +1669,10 @@
         <v>3</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="4" t="s">
         <v>4</v>
       </c>
@@ -1596,64 +1681,64 @@
       </c>
       <c r="C89" s="4"/>
     </row>
-    <row r="90" spans="1:3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B90" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B90" s="4" t="s">
+      <c r="C90" s="4"/>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C90" s="4"/>
-    </row>
-    <row r="91" spans="1:3">
-      <c r="A91" s="4" t="s">
-        <v>13</v>
-      </c>
       <c r="B91" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C91" s="4"/>
     </row>
-    <row r="92" spans="1:3" ht="51">
+    <row r="92" spans="1:3" ht="42.75" x14ac:dyDescent="0.3">
       <c r="A92" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B92" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C92" s="7"/>
+    </row>
+    <row r="93" spans="1:3" ht="28.5" x14ac:dyDescent="0.3">
+      <c r="A93" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B93" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B92" s="8" t="s">
+      <c r="C93" s="7"/>
+    </row>
+    <row r="94" spans="1:3" ht="28.5" x14ac:dyDescent="0.3">
+      <c r="B94" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C92" s="7"/>
-    </row>
-    <row r="93" spans="1:3">
-      <c r="A93" s="8" t="s">
+      <c r="C94" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B93" s="8" t="s">
+    </row>
+    <row r="95" spans="1:3" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="C93" s="7"/>
-    </row>
-    <row r="94" spans="1:3" ht="15" customHeight="1">
-      <c r="B94" s="8" t="s">
+      <c r="B95" s="20"/>
+      <c r="C95" s="10"/>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A97" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C94" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" ht="32.25" customHeight="1">
-      <c r="A95" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="B95" s="18"/>
-      <c r="C95" s="10"/>
-    </row>
-    <row r="97" spans="1:3">
-      <c r="A97" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="B97" s="3"/>
     </row>
-    <row r="98" spans="1:3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" s="4" t="s">
         <v>2</v>
       </c>
@@ -1661,10 +1746,10 @@
         <v>3</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" s="4" t="s">
         <v>4</v>
       </c>
@@ -1673,59 +1758,59 @@
       </c>
       <c r="C99" s="4"/>
     </row>
-    <row r="100" spans="1:3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B100" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B100" s="4" t="s">
+      <c r="C100" s="4"/>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A101" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C100" s="4"/>
-    </row>
-    <row r="101" spans="1:3">
-      <c r="A101" s="4" t="s">
-        <v>13</v>
-      </c>
       <c r="B101" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C101" s="4"/>
     </row>
-    <row r="102" spans="1:3" ht="34.5">
+    <row r="102" spans="1:5" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A102" s="8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C102" s="8"/>
     </row>
-    <row r="103" spans="1:3" ht="34.5">
+    <row r="103" spans="1:5" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A103" s="8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C103" s="20"/>
-    </row>
-    <row r="104" spans="1:3" ht="18" customHeight="1">
+        <v>112</v>
+      </c>
+      <c r="C103" s="17"/>
+    </row>
+    <row r="104" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="8"/>
       <c r="B104" s="8" t="s">
-        <v>72</v>
+        <v>113</v>
       </c>
       <c r="C104" s="8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" s="12" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B106" s="13"/>
       <c r="C106" s="14"/>
     </row>
-    <row r="107" spans="1:3">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" s="15" t="s">
         <v>2</v>
       </c>
@@ -1733,391 +1818,435 @@
         <v>3</v>
       </c>
       <c r="C107" s="15" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3">
+        <v>109</v>
+      </c>
+      <c r="D107" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="E107" s="25" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" s="15" t="s">
         <v>4</v>
       </c>
       <c r="B108" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C108" s="15"/>
-    </row>
-    <row r="109" spans="1:3">
+      <c r="C108" s="22"/>
+      <c r="D108" s="26"/>
+      <c r="E108" s="26"/>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B109" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B109" s="15" t="s">
+      <c r="C109" s="22"/>
+      <c r="D109" s="26"/>
+      <c r="E109" s="26"/>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A110" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C109" s="15"/>
-    </row>
-    <row r="110" spans="1:3">
-      <c r="A110" s="15" t="s">
+      <c r="B110" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B110" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C110" s="15"/>
-    </row>
-    <row r="111" spans="1:3">
+      <c r="C110" s="22"/>
+      <c r="D110" s="26"/>
+      <c r="E110" s="26"/>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B111" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C111" s="23"/>
+      <c r="D111" s="26"/>
+      <c r="E111" s="26"/>
+    </row>
+    <row r="112" spans="1:5" ht="28.5" x14ac:dyDescent="0.3">
+      <c r="A112" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B112" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="C112" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="D112" s="26"/>
+      <c r="E112" s="26"/>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A113" s="7"/>
+      <c r="B113" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C113" s="24"/>
+      <c r="D113" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="E113" s="26"/>
+    </row>
+    <row r="114" spans="1:5" ht="28.5" x14ac:dyDescent="0.3">
+      <c r="A114" s="7"/>
+      <c r="B114" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C114" s="24"/>
+      <c r="D114" s="21"/>
+      <c r="E114" s="26"/>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A115" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B115" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C115" s="24"/>
+      <c r="D115" s="26"/>
+      <c r="E115" s="21" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="42.75" x14ac:dyDescent="0.3">
+      <c r="A116" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="B116" s="16"/>
+      <c r="C116" s="23"/>
+      <c r="D116" s="26"/>
+      <c r="E116" s="26"/>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A118" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B118" s="3"/>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A119" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B119" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A120" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B120" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A121" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B121" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A122" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B122" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" ht="28.5" x14ac:dyDescent="0.3">
+      <c r="A123" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B123" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B124" s="7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B111" s="16" t="s">
+      <c r="B125" s="8"/>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A127" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C111" s="16"/>
-    </row>
-    <row r="112" spans="1:3" ht="34.5">
-      <c r="A112" s="16" t="s">
+      <c r="B127" s="3"/>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A128" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B128" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A129" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B129" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A130" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B130" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A131" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B131" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A132" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="B112" s="16" t="s">
+      <c r="B132" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="C112" s="16"/>
-    </row>
-    <row r="113" spans="1:3">
-      <c r="A113" s="16" t="s">
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A134" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B113" s="16"/>
-      <c r="C113" s="16" t="s">
+      <c r="B134" s="3"/>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A135" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B135" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A136" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B136" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A137" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B137" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A138" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B138" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A139" s="8" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" ht="51">
-      <c r="A114" s="16" t="s">
+      <c r="B139" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="B114" s="16"/>
-      <c r="C114" s="16"/>
-    </row>
-    <row r="116" spans="1:3">
-      <c r="A116" s="2" t="s">
+    </row>
+    <row r="140" spans="1:2" ht="71.25" x14ac:dyDescent="0.3">
+      <c r="A140" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="B116" s="3"/>
-    </row>
-    <row r="117" spans="1:3">
-      <c r="A117" s="4" t="s">
+      <c r="B140" s="11"/>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A142" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B142" s="3"/>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A143" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B117" s="4" t="s">
+      <c r="B143" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="118" spans="1:3">
-      <c r="A118" s="4" t="s">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A144" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B144" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A146" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B146" s="3"/>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A147" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B147" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A148" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B148" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A150" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B150" s="3"/>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A151" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B151" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A152" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B118" s="4" t="s">
+      <c r="B152" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="119" spans="1:3">
-      <c r="A119" s="4" t="s">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A153" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B153" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B119" s="4" t="s">
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A154" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="120" spans="1:3">
-      <c r="A120" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B120" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" ht="34.5">
-      <c r="A121" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="B121" s="8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" ht="39" customHeight="1">
-      <c r="A122" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="B122" s="7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" ht="33" customHeight="1">
-      <c r="A123" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="B123" s="8"/>
-    </row>
-    <row r="125" spans="1:3">
-      <c r="A125" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B125" s="3"/>
-    </row>
-    <row r="126" spans="1:3">
-      <c r="A126" s="4" t="s">
+      <c r="B154" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A155" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B155" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A156" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B156" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" ht="42.75" x14ac:dyDescent="0.3">
+      <c r="A157" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B157" s="11"/>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A159" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B159" s="3"/>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A160" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B126" s="4" t="s">
+      <c r="B160" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="127" spans="1:3">
-      <c r="A127" s="4" t="s">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A161" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B127" s="4" t="s">
+      <c r="B161" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="128" spans="1:3">
-      <c r="A128" s="4" t="s">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A162" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B162" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B128" s="4" t="s">
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A163" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="129" spans="1:2">
-      <c r="A129" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B129" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2">
-      <c r="A130" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="B130" s="7" t="s">
+      <c r="B163" s="4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="132" spans="1:2">
-      <c r="A132" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B132" s="3"/>
-    </row>
-    <row r="133" spans="1:2">
-      <c r="A133" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B133" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2">
-      <c r="A134" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B134" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2">
-      <c r="A135" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B135" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2">
-      <c r="A136" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B136" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" ht="51" customHeight="1">
-      <c r="A137" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="B137" s="8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" ht="85.5">
-      <c r="A138" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="B138" s="11"/>
-    </row>
-    <row r="140" spans="1:2">
-      <c r="A140" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B140" s="3"/>
-    </row>
-    <row r="141" spans="1:2">
-      <c r="A141" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B141" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2">
-      <c r="A142" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B142" s="4" t="s">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A164" s="8" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="144" spans="1:2">
-      <c r="A144" s="2" t="s">
+      <c r="B164" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="B144" s="3"/>
-    </row>
-    <row r="145" spans="1:2">
-      <c r="A145" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B145" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2">
-      <c r="A146" s="4" t="s">
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A165" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="B146" s="4" t="s">
+      <c r="B165" s="8" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="148" spans="1:2">
-      <c r="A148" s="2" t="s">
+    <row r="166" spans="1:2" ht="42.75" x14ac:dyDescent="0.3">
+      <c r="A166" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="B148" s="3"/>
-    </row>
-    <row r="149" spans="1:2">
-      <c r="A149" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B149" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2">
-      <c r="A150" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B150" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2">
-      <c r="A151" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B151" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2">
-      <c r="A152" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B152" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2">
-      <c r="A153" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="B153" s="8" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" ht="34.5" customHeight="1">
-      <c r="A154" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="B154" s="8" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" ht="51">
-      <c r="A155" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="B155" s="11"/>
-    </row>
-    <row r="157" spans="1:2">
-      <c r="A157" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B157" s="3"/>
-    </row>
-    <row r="158" spans="1:2">
-      <c r="A158" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B158" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2">
-      <c r="A159" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B159" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2">
-      <c r="A160" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B160" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2">
-      <c r="A161" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B161" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2">
-      <c r="A162" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="B162" s="8" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" ht="33" customHeight="1">
-      <c r="A163" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="B163" s="8" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" ht="51">
-      <c r="A164" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="B164" s="8"/>
+      <c r="B166" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2125,6 +2254,7 @@
     <mergeCell ref="A69:B69"/>
     <mergeCell ref="A95:B95"/>
   </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>